<commit_message>
Metabolite label uploads, bootstrap data adjustment
</commit_message>
<xml_diff>
--- a/scripts/bootstrap/measurement_data/synthetic_gut.xlsx
+++ b/scripts/bootstrap/measurement_data/synthetic_gut.xlsx
@@ -129,7 +129,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Abundances values per time-point for strain Roseburia intestinalis L1-82, use a period (.) as the decimal separator.</t>
+          <t xml:space="preserve">FC counts values per time-point for strain Roseburia intestinalis L1-82 in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
       </text>
     </comment>
@@ -153,7 +153,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Abundances values per time-point for strain Blautia hydrogenotrophica DSM 10507, use a period (.) as the decimal separator.</t>
+          <t xml:space="preserve">FC counts values per time-point for strain Blautia hydrogenotrophica DSM 10507 in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
       </text>
     </comment>
@@ -177,7 +177,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Abundances values per time-point for strain Prevotella copri DSM 18205, use a period (.) as the decimal separator.</t>
+          <t xml:space="preserve">FC counts values per time-point for strain Prevotella copri DSM 18205 in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
       </text>
     </comment>
@@ -201,7 +201,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Abundances values per time-point for strain Bacteroides thetaiotaomicron VPI-5482, use a period (.) as the decimal separator.</t>
+          <t xml:space="preserve">FC counts values per time-point for strain Bacteroides thetaiotaomicron VPI-5482 in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
       </text>
     </comment>
@@ -225,7 +225,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Abundances values per time-point for strain Collinsella aerofaciens RCC 1377, use a period (.) as the decimal separator.</t>
+          <t xml:space="preserve">FC counts values per time-point for strain Collinsella aerofaciens RCC 1377 in Cells/mL, use a period (.) as the decimal separator</t>
         </r>
       </text>
     </comment>
@@ -436,7 +436,7 @@
     <t xml:space="preserve">Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Community FC</t>
+    <t xml:space="preserve">Community FC (ML)</t>
   </si>
   <si>
     <t xml:space="preserve">biorep1</t>
@@ -460,34 +460,34 @@
     <t xml:space="preserve">biorep6</t>
   </si>
   <si>
-    <t xml:space="preserve">Roseburia intestinalis L1-82 rRNA reads</t>
+    <t xml:space="preserve">Roseburia intestinalis L1-82 FC counts (16S)</t>
   </si>
   <si>
-    <t xml:space="preserve">Roseburia intestinalis L1-82 rRNA reads STD</t>
+    <t xml:space="preserve">Roseburia intestinalis L1-82 FC counts (16S) STD</t>
   </si>
   <si>
-    <t xml:space="preserve">Blautia hydrogenotrophica DSM 10507 rRNA reads</t>
+    <t xml:space="preserve">Blautia hydrogenotrophica DSM 10507 FC counts (16S)</t>
   </si>
   <si>
-    <t xml:space="preserve">Blautia hydrogenotrophica DSM 10507 rRNA reads STD</t>
+    <t xml:space="preserve">Blautia hydrogenotrophica DSM 10507 FC counts (16S) STD</t>
   </si>
   <si>
-    <t xml:space="preserve">Prevotella copri DSM 18205 rRNA reads</t>
+    <t xml:space="preserve">Prevotella copri DSM 18205 FC counts (16S)</t>
   </si>
   <si>
-    <t xml:space="preserve">Prevotella copri DSM 18205 rRNA reads STD</t>
+    <t xml:space="preserve">Prevotella copri DSM 18205 FC counts (16S) STD</t>
   </si>
   <si>
-    <t xml:space="preserve">Bacteroides thetaiotaomicron VPI-5482 rRNA reads</t>
+    <t xml:space="preserve">Bacteroides thetaiotaomicron VPI-5482 FC counts (16S)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bacteroides thetaiotaomicron VPI-5482 rRNA reads STD</t>
+    <t xml:space="preserve">Bacteroides thetaiotaomicron VPI-5482 FC counts (16S) STD</t>
   </si>
   <si>
-    <t xml:space="preserve">Collinsella aerofaciens RCC 1377 rRNA reads</t>
+    <t xml:space="preserve">Collinsella aerofaciens RCC 1377 FC counts (16S)</t>
   </si>
   <si>
-    <t xml:space="preserve">Collinsella aerofaciens RCC 1377 rRNA reads STD</t>
+    <t xml:space="preserve">Collinsella aerofaciens RCC 1377 FC counts (16S) STD</t>
   </si>
   <si>
     <t xml:space="preserve">pyruvate</t>
@@ -939,11 +939,11 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="D38" activeCellId="1" sqref="F1:G1 D38"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="1" sqref="F1:G1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -951,7 +951,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,10 +1498,10 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
@@ -1510,8 +1510,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="41.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.6"/>
@@ -1532,10 +1532,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -1544,10 +1544,10 @@
       <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -1556,10 +1556,10 @@
       <c r="K1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>